<commit_message>
More than half complete for a draft
</commit_message>
<xml_diff>
--- a/review paper/Links.xlsx
+++ b/review paper/Links.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\smit\Review Paper\Review-Paper_ARIMA-Model\review paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB960B36-2C01-4F9B-87BA-A4B758D09C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A195986-C4CF-4AC2-8E05-123578EF9B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12103" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11614" yWindow="1277" windowWidth="8760" windowHeight="10157" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReviewPaper" sheetId="1" r:id="rId1"/>
-    <sheet name="Colleges" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Colleges" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t xml:space="preserve">Author </t>
   </si>
@@ -139,6 +140,48 @@
   </si>
   <si>
     <t>Kyoung-jae Kim</t>
+  </si>
+  <si>
+    <t>ANN</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S2314728817300715</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1877050915006766</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/318127667_Forecasting_of_nonlinear_time_series_using_ANN</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>ARIMA</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=vb9EOUMAAAAJ&amp;hl=it</t>
+  </si>
+  <si>
+    <t>https://www.tableau.com/learn/articles/time-series-forecasting</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?view_op=view_citation&amp;hl=it&amp;user=vb9EOUMAAAAJ&amp;citation_for_view=vb9EOUMAAAAJ:HeT0ZceujKMC</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/222661136_Financial_time_series_forecasting_using_support_vector_machines</t>
+  </si>
+  <si>
+    <t>https://sci-hub.mksa.top/10.1016/s0925-2312(03)00372-2</t>
+  </si>
+  <si>
+    <t>https://www.analyticssteps.com/blogs/how-does-support-vector-machine-algorithm-works-machine-learning</t>
+  </si>
+  <si>
+    <t>In-Depth: Support Vector Machines | Python Data Science Handbook (jakevdp.github.io)</t>
   </si>
 </sst>
 </file>
@@ -501,10 +544,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" customHeight="1"/>
@@ -643,6 +686,26 @@
       </c>
       <c r="B14" s="14" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A23" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -666,6 +729,150 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC16A559-2FDA-4CEB-AEF5-10F7FADB06CA}">
+  <dimension ref="A1:A27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.45"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A12" r:id="rId1" xr:uid="{44F096C8-FD5F-4896-ADE5-AFC165327CCC}"/>
+    <hyperlink ref="A16" r:id="rId2" xr:uid="{430A5F9E-E6E4-493B-822F-E765B1E36E11}"/>
+    <hyperlink ref="A15" r:id="rId3" xr:uid="{B4B31A59-82A9-4994-BA73-80A8392F9944}"/>
+    <hyperlink ref="A14" r:id="rId4" xr:uid="{097DEBA1-6DF1-4284-97CA-B8ECA74544BD}"/>
+    <hyperlink ref="A13" r:id="rId5" xr:uid="{3DAC5AF2-0385-4354-8B25-EA0F22B49147}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{E1685A7A-BA20-426F-8D89-363839755F99}"/>
+    <hyperlink ref="A7" r:id="rId7" xr:uid="{6F72EF91-95D2-4B80-BE56-731EE38C96B0}"/>
+    <hyperlink ref="A4" r:id="rId8" xr:uid="{10B982D3-6B34-4B82-A3EF-B82F2DE1CB47}"/>
+    <hyperlink ref="A3" r:id="rId9" xr:uid="{356671BD-6DAE-4F8C-8DEC-3B326C8F0FA0}"/>
+    <hyperlink ref="A2" r:id="rId10" xr:uid="{D79F33BD-9D68-4C00-968D-1E6DEF42DF6E}"/>
+    <hyperlink ref="A20" r:id="rId11" xr:uid="{97E1CAF1-BD04-46D9-B7E1-76D6DDD094C6}"/>
+    <hyperlink ref="A21" r:id="rId12" xr:uid="{AC15248F-39AB-4999-BFCC-37908C3AD64B}"/>
+    <hyperlink ref="A22" r:id="rId13" xr:uid="{8F9EC165-92C3-43BB-A594-629C8DA10B66}"/>
+    <hyperlink ref="A23" r:id="rId14" xr:uid="{4BF3659A-2F67-486B-8F84-A67E7CC88B4A}"/>
+    <hyperlink ref="A26" r:id="rId15" xr:uid="{6A23205A-BAC7-48DE-935A-D6E15C0EBCC6}"/>
+    <hyperlink ref="A27" r:id="rId16" xr:uid="{B6A940A6-09B4-47E9-9F14-5C948BAA25AA}"/>
+    <hyperlink ref="A17" r:id="rId17" display="https://jakevdp.github.io/PythonDataScienceHandbook/05.07-support-vector-machines.html" xr:uid="{93821CCC-03C1-49AC-82A0-B89BE6460DD1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
ANN sarkhu karvanu he baki
</commit_message>
<xml_diff>
--- a/review paper/Links.xlsx
+++ b/review paper/Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\smit\Review Paper\Review-Paper_ARIMA-Model\review paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A195986-C4CF-4AC2-8E05-123578EF9B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DF9457-12CA-485C-9D30-9AD70BB46BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11614" yWindow="1277" windowWidth="8760" windowHeight="10157" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t xml:space="preserve">Author </t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>In-Depth: Support Vector Machines | Python Data Science Handbook (jakevdp.github.io)</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/228379704_New_ARIMA_Models_for_Seasonal_Time_Series_and_Their_Application_to_Seasonal_Adjustment_and_Forecasting</t>
   </si>
 </sst>
 </file>
@@ -732,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC16A559-2FDA-4CEB-AEF5-10F7FADB06CA}">
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A24" sqref="A19:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45"/>
@@ -771,6 +774,11 @@
     <row r="8" spans="1:1">
       <c r="A8" s="14" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:1">
@@ -867,6 +875,7 @@
     <hyperlink ref="A26" r:id="rId15" xr:uid="{6A23205A-BAC7-48DE-935A-D6E15C0EBCC6}"/>
     <hyperlink ref="A27" r:id="rId16" xr:uid="{B6A940A6-09B4-47E9-9F14-5C948BAA25AA}"/>
     <hyperlink ref="A17" r:id="rId17" display="https://jakevdp.github.io/PythonDataScienceHandbook/05.07-support-vector-machines.html" xr:uid="{93821CCC-03C1-49AC-82A0-B89BE6460DD1}"/>
+    <hyperlink ref="A9" r:id="rId18" xr:uid="{DD52D9A9-4BC9-4265-A7DE-689009E116FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new photos and formatting
</commit_message>
<xml_diff>
--- a/review paper/Links.xlsx
+++ b/review paper/Links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\smit\Review Paper\Review-Paper_ARIMA-Model\review paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD2A69E-967C-4E31-BBAA-C0EDE60C6F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92001E18-A159-4B66-9BA6-21AE8197EC91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12103" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11614" yWindow="1277" windowWidth="8760" windowHeight="10157" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReviewPaper" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t xml:space="preserve">Author </t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>https://www.researchgate.net/publication/228379704_New_ARIMA_Models_for_Seasonal_Time_Series_and_Their_Application_to_Seasonal_Adjustment_and_Forecasting</t>
+  </si>
+  <si>
+    <t>Inference robustness of ARIMA models under non-normality —Special application to stock price data | SpringerLink</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -733,10 +736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC16A559-2FDA-4CEB-AEF5-10F7FADB06CA}">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45"/>
@@ -854,6 +857,11 @@
     <row r="27" spans="1:1">
       <c r="A27" s="14" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -876,6 +884,7 @@
     <hyperlink ref="A27" r:id="rId16" xr:uid="{B6A940A6-09B4-47E9-9F14-5C948BAA25AA}"/>
     <hyperlink ref="A17" r:id="rId17" display="https://jakevdp.github.io/PythonDataScienceHandbook/05.07-support-vector-machines.html" xr:uid="{93821CCC-03C1-49AC-82A0-B89BE6460DD1}"/>
     <hyperlink ref="A9" r:id="rId18" xr:uid="{DD52D9A9-4BC9-4265-A7DE-689009E116FB}"/>
+    <hyperlink ref="A31" r:id="rId19" display="https://link.springer.com/article/10.1007/BF01893469" xr:uid="{CB3DFBCC-B15A-4306-8BC0-083362C43C92}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
kale submit, have a good night ishan
</commit_message>
<xml_diff>
--- a/review paper/Links.xlsx
+++ b/review paper/Links.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\smit\Review Paper\Review-Paper_ARIMA-Model\review paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92001E18-A159-4B66-9BA6-21AE8197EC91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781B0AB6-44E8-41E2-B58F-7E145EB417DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11614" yWindow="1277" windowWidth="8760" windowHeight="10157" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12103" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReviewPaper" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="Colleges" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Journals" sheetId="4" r:id="rId3"/>
+    <sheet name="Colleges" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t xml:space="preserve">Author </t>
   </si>
@@ -188,6 +189,24 @@
   </si>
   <si>
     <t>Inference robustness of ARIMA models under non-normality —Special application to stock price data | SpringerLink</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/sourceid/26132</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/sourceid/12140</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/sourceid/21100466714</t>
+  </si>
+  <si>
+    <t>https://thescipub.com/jcs/about</t>
+  </si>
+  <si>
+    <t>IRJMETS- Journal with 599 Rs. publication fees | In 4 hr paper published | Low cost journal | Engineering | Scientific journal</t>
+  </si>
+  <si>
+    <t>https://www.scopus.com/sourceid/21100466714#tabs=2</t>
   </si>
 </sst>
 </file>
@@ -738,7 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC16A559-2FDA-4CEB-AEF5-10F7FADB06CA}">
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -891,6 +910,63 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAC218D-201D-4F38-A178-9428D2F8AD10}">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.45"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1" display="https://www.irjmets.com/?gclid=Cj0KCQjwlN" xr:uid="{DC333AB3-72E1-4F1B-A97D-3D1B30033E36}"/>
+    <hyperlink ref="A1" r:id="rId2" xr:uid="{4004342E-F7FB-41C6-98C8-3FCA094261E7}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{E0E83051-3DBE-49EB-99C7-09D8220F3403}"/>
+    <hyperlink ref="A7" r:id="rId4" xr:uid="{E394E6F5-F732-4477-9052-8552A7AA621D}"/>
+    <hyperlink ref="A12" r:id="rId5" location="tabs=2" xr:uid="{38883312-51E2-47CB-96FC-D85179C5F89B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>